<commit_message>
Finished to Import Excel
</commit_message>
<xml_diff>
--- a/uploads/Caneva_SecretariatMedical10.xlsx
+++ b/uploads/Caneva_SecretariatMedical10.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="60" windowWidth="12915" windowHeight="11025" activeTab="3"/>
+    <workbookView xWindow="600" yWindow="60" windowWidth="12915" windowHeight="11025" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ChoixMultiples" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="237">
   <si>
     <t>Questions</t>
   </si>
@@ -473,9 +473,6 @@
   </si>
   <si>
     <t>kilo</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> simple</t>
   </si>
   <si>
     <t>Inserez la définitions et les extensions</t>
@@ -1300,10 +1297,10 @@
   <sheetData>
     <row r="1" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" s="33" t="s">
         <v>215</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>216</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="33"/>
@@ -1478,13 +1475,13 @@
   <sheetData>
     <row r="1" spans="1:9" s="18" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="34" t="s">
         <v>213</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>214</v>
       </c>
       <c r="D1" s="34"/>
       <c r="E1" s="34"/>
@@ -1591,13 +1588,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>217</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1739,7 +1736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1752,13 +1749,13 @@
   <sheetData>
     <row r="1" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>221</v>
-      </c>
       <c r="C1" s="35" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D1" s="35"/>
       <c r="E1" s="35"/>
@@ -1815,7 +1812,7 @@
         <v>86</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1823,7 +1820,7 @@
         <v>72</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>87</v>
@@ -1896,8 +1893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,10 +1906,10 @@
   <sheetData>
     <row r="1" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
@@ -1924,25 +1921,25 @@
         <v>104</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -1975,7 +1972,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="B4" t="s">
         <v>106</v>
@@ -2066,7 +2063,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B8" t="s">
         <v>58</v>
@@ -2138,22 +2135,22 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="38" t="s">
         <v>155</v>
-      </c>
-      <c r="F11" s="38" t="s">
-        <v>156</v>
       </c>
       <c r="G11" s="38"/>
       <c r="H11" s="38"/>
@@ -2162,22 +2159,22 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E12" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>159</v>
-      </c>
       <c r="F12" s="37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
@@ -2186,19 +2183,19 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" t="s">
         <v>162</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>163</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>165</v>
-      </c>
       <c r="F13" s="37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G13" s="37"/>
       <c r="H13" s="37"/>
@@ -2207,19 +2204,19 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C14" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14" t="s">
         <v>166</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="E14" s="14" t="s">
-        <v>168</v>
-      </c>
       <c r="F14" s="37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
@@ -2228,19 +2225,19 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C15" t="s">
         <v>170</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>171</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F15" s="37" t="s">
         <v>172</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="F15" s="37" t="s">
-        <v>173</v>
       </c>
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
@@ -2277,10 +2274,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>233</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2288,39 +2285,39 @@
         <v>0</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2349,13 +2346,13 @@
   <sheetData>
     <row r="1" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B1" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>235</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>236</v>
       </c>
       <c r="D1" s="36"/>
       <c r="E1" s="36"/>
@@ -2369,7 +2366,7 @@
         <v>104</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>75</v>
@@ -2404,10 +2401,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
         <v>108</v>
@@ -2430,30 +2427,30 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" t="s">
         <v>190</v>
       </c>
-      <c r="D4" t="s">
-        <v>191</v>
-      </c>
       <c r="E4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G4" t="s">
         <v>193</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>194</v>
-      </c>
-      <c r="H4" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2473,27 +2470,27 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E6" t="s">
         <v>198</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>199</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>200</v>
-      </c>
-      <c r="G6" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B7" t="s">
         <v>204</v>
-      </c>
-      <c r="B7" t="s">
-        <v>205</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2516,22 +2513,22 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D8" t="s">
         <v>206</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>207</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>208</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>209</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>210</v>
-      </c>
-      <c r="H8" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>